<commit_message>
[POI4] 0.5.1: Now ready to start with apache poi 4.1.2.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoStringGroupConstants.xlsx
+++ b/meta/program/BlancoStringGroupConstants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoStringGroup/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0280318D-6603-8C4D-92DB-ABC66B9C8296}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB7552F6-A030-F247-B9AB-34495B13B713}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20940" yWindow="6660" windowWidth="17140" windowHeight="14600" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16460" yWindow="6400" windowWidth="17140" windowHeight="14600" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -239,7 +239,7 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>"2.1.1"</t>
+    <t>"0.5.1"</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -1111,7 +1111,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>

</xml_diff>